<commit_message>
Declaring sub-genotype reference sequences and creating corresponding alignments
</commit_message>
<xml_diff>
--- a/tabular/hbv_refseq_data.xlsx
+++ b/tabular/hbv_refseq_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9880" yWindow="0" windowWidth="36420" windowHeight="24720" tabRatio="500"/>
+    <workbookView xWindow="460" yWindow="2460" windowWidth="30300" windowHeight="20820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1054,8 +1054,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1116,7 +1174,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1136,6 +1194,35 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1155,6 +1242,35 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1487,7 +1603,7 @@
   <dimension ref="A1:S69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Validated max-likelihood genotyping at genotype level
</commit_message>
<xml_diff>
--- a/tabular/hbv_refseq_data.xlsx
+++ b/tabular/hbv_refseq_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="2460" windowWidth="30300" windowHeight="20820" tabRatio="500"/>
+    <workbookView xWindow="14580" yWindow="740" windowWidth="30300" windowHeight="20820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1602,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Extending alignment tree to enable genotyping to subgenotype level
</commit_message>
<xml_diff>
--- a/tabular/hbv_refseq_data.xlsx
+++ b/tabular/hbv_refseq_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="740" windowWidth="30300" windowHeight="20820" tabRatio="500"/>
+    <workbookView xWindow="17960" yWindow="0" windowWidth="30300" windowHeight="20820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1602,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="E16:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updated genotyping to assign at genotype level only (subgenotypes inconsistent with tree)
</commit_message>
<xml_diff>
--- a/tabular/hbv_refseq_data.xlsx
+++ b/tabular/hbv_refseq_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17960" yWindow="0" windowWidth="30300" windowHeight="20820" tabRatio="500"/>
+    <workbookView xWindow="17960" yWindow="0" windowWidth="31220" windowHeight="25580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -995,7 +995,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1044,6 +1044,18 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1054,7 +1066,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1152,8 +1164,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1173,8 +1191,10 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1223,6 +1243,9 @@
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1271,6 +1294,9 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1602,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="E16:G20"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2794,10 +2820,10 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C21">
         <v>3182</v>
@@ -2818,7 +2844,7 @@
         <v>117</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="J21" t="s">
         <v>115</v>
@@ -2853,19 +2879,19 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C22">
         <v>3182</v>
       </c>
       <c r="D22" s="9">
-        <v>40756</v>
+        <v>40966</v>
       </c>
       <c r="E22" s="9">
-        <v>40756</v>
+        <v>42807</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>39</v>
@@ -2877,28 +2903,28 @@
         <v>117</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="J22" t="s">
         <v>115</v>
       </c>
       <c r="K22">
-        <v>21678435</v>
+        <v>22785194</v>
       </c>
       <c r="L22" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="M22" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="N22" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="O22" t="s">
         <v>115</v>
       </c>
-      <c r="P22" t="s">
-        <v>115</v>
+      <c r="P22">
+        <v>2010</v>
       </c>
       <c r="Q22" t="s">
         <v>115</v>
@@ -2907,24 +2933,24 @@
         <v>115</v>
       </c>
       <c r="S22">
-        <v>21678435</v>
+        <v>22785194</v>
       </c>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C23">
         <v>3182</v>
       </c>
       <c r="D23" s="9">
-        <v>40966</v>
+        <v>40756</v>
       </c>
       <c r="E23" s="9">
-        <v>42807</v>
+        <v>40756</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>39</v>
@@ -2936,28 +2962,28 @@
         <v>117</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="J23" t="s">
         <v>115</v>
       </c>
       <c r="K23">
-        <v>22785194</v>
+        <v>21678435</v>
       </c>
       <c r="L23" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="M23" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="N23" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="O23" t="s">
         <v>115</v>
       </c>
-      <c r="P23">
-        <v>2010</v>
+      <c r="P23" t="s">
+        <v>115</v>
       </c>
       <c r="Q23" t="s">
         <v>115</v>
@@ -2966,7 +2992,7 @@
         <v>115</v>
       </c>
       <c r="S23">
-        <v>22785194</v>
+        <v>21678435</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -3457,10 +3483,10 @@
       <c r="E32" s="9">
         <v>40002</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="13" t="s">
         <v>52</v>
       </c>
       <c r="H32" t="s">
@@ -4327,10 +4353,10 @@
       </c>
     </row>
     <row r="47" spans="1:19">
-      <c r="A47" t="s">
+      <c r="A47" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="14" t="s">
         <v>151</v>
       </c>
       <c r="C47">
@@ -4386,10 +4412,10 @@
       </c>
     </row>
     <row r="48" spans="1:19">
-      <c r="A48" t="s">
+      <c r="A48" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="14" t="s">
         <v>156</v>
       </c>
       <c r="C48">
@@ -4445,10 +4471,10 @@
       </c>
     </row>
     <row r="49" spans="1:19">
-      <c r="A49" t="s">
+      <c r="A49" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="14" t="s">
         <v>263</v>
       </c>
       <c r="C49">
@@ -4504,10 +4530,10 @@
       </c>
     </row>
     <row r="50" spans="1:19">
-      <c r="A50" t="s">
+      <c r="A50" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="14" t="s">
         <v>265</v>
       </c>
       <c r="C50">
@@ -4563,10 +4589,10 @@
       </c>
     </row>
     <row r="51" spans="1:19">
-      <c r="A51" t="s">
+      <c r="A51" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="14" t="s">
         <v>271</v>
       </c>
       <c r="C51">
@@ -4622,10 +4648,10 @@
       </c>
     </row>
     <row r="52" spans="1:19">
-      <c r="A52" t="s">
+      <c r="A52" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="14" t="s">
         <v>294</v>
       </c>
       <c r="C52">

</xml_diff>